<commit_message>
Fix the connection to the MongoDB with IPv4 and the import from Excel data into MongoDB
</commit_message>
<xml_diff>
--- a/backend/util/lab_instruments.xlsx
+++ b/backend/util/lab_instruments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giggi\OneDrive\Desktop\shared\NodeJS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\lab-booking-system-master\lab-booking-system-master\backend\util\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72189368-7028-4357-850E-A5FFDAF6D3FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CD7C94-50E6-49CE-9268-E3791B451A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{103AE25C-D4A2-4EE3-94AB-DBD333D31CE9}"/>
   </bookViews>

</xml_diff>